<commit_message>
bunnies analysis, models and summary
</commit_message>
<xml_diff>
--- a/models-summary.xlsx
+++ b/models-summary.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\School\more adjs\experiment 1b\analysis-all\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998D9150-02CD-42DE-A939-24D39DC4ADA3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A988B90-E689-48FF-A3C2-BBEE08C47E80}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="685" xr2:uid="{BE17DB3E-6EB1-4E46-A183-F9B0FC02F479}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="685" activeTab="1" xr2:uid="{BE17DB3E-6EB1-4E46-A183-F9B0FC02F479}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
     <sheet name="z score summary" sheetId="14" r:id="rId2"/>
     <sheet name="rep - are" sheetId="2" r:id="rId3"/>
     <sheet name="m.allvs.simp" sheetId="3" r:id="rId4"/>
-    <sheet name="m.rev" sheetId="5" r:id="rId5"/>
-    <sheet name="m.ordphot" sheetId="13" r:id="rId6"/>
-    <sheet name="m.ranphot" sheetId="7" r:id="rId7"/>
-    <sheet name="m.rantiny" sheetId="8" r:id="rId8"/>
+    <sheet name="m.bunny" sheetId="15" r:id="rId5"/>
+    <sheet name="m.rev" sheetId="5" r:id="rId6"/>
+    <sheet name="m.ordphot" sheetId="13" r:id="rId7"/>
+    <sheet name="m.ranphot" sheetId="7" r:id="rId8"/>
+    <sheet name="m.rantiny" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="593">
   <si>
     <t>experiment</t>
   </si>
@@ -1471,6 +1472,357 @@
   </si>
   <si>
     <t>though barely</t>
+  </si>
+  <si>
+    <t>bunnies-cartoons</t>
+  </si>
+  <si>
+    <t>m.bunny</t>
+  </si>
+  <si>
+    <t>clmm(fac_num_checked ~ adj*prototype_status + dir + quest_order + (1+adj|noun) + (1+adj*prototype_status|subid), data=d.bunny)</t>
+  </si>
+  <si>
+    <t>m.bunny.simple</t>
+  </si>
+  <si>
+    <t>clmm(fac_num_checked ~ adj*prototype_status + dir + quest_order + (1+adj|noun) + (1|subid), data=d.bunny)</t>
+  </si>
+  <si>
+    <t>m.bunny.norm</t>
+  </si>
+  <si>
+    <t>clmm(fac_num_checked ~ adj*mean + dir + quest_order + (1+adj|noun) + (1+adj|subid), data=d.bunny)</t>
+  </si>
+  <si>
+    <t>m.bunny.relev</t>
+  </si>
+  <si>
+    <t>clmm(fac_num_checked ~ adj*protr + dir + quest_order + (1+adj|noun) + (1+adj*protr|subid), data=d.bunny)</t>
+  </si>
+  <si>
+    <t>not significant</t>
+  </si>
+  <si>
+    <t>data:    d.bunny</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> logit flexible  2087 -1269.63 2613.26 6560(64537) 1.32e-02 3.3e+09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Groups Name                             Variance Std.Dev. Corr                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> subid  (Intercept)                      20.9576  4.5779                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall                         37.4248  6.1176   -0.442                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        prototype_statusneither           0.1792  0.4233    0.023  0.887              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        prototype_statussmall             2.8815  1.6975   -0.278  0.789  0.736       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall:prototype_statusneither  0.8109  0.9005    0.355 -0.934 -0.858 -0.956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall:prototype_statussmall   11.2310  3.3513    0.433 -0.753 -0.616 -0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> noun   (Intercept)                       0.2674  0.5171                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall                          0.8411  0.9171   -1.000                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of groups:  subid 44,  noun 12 </t>
+  </si>
+  <si>
+    <t>adjsmall                          5.772892   1.068225   5.404 6.51e-08 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prototype_statusneither           0.407304   0.440299   0.925  0.35493    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prototype_statussmall             1.088610   0.506879   2.148  0.03174 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dirdesc                          -0.082658   0.116840  -0.707  0.47929    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quest_order                       0.004404   0.004356   1.011  0.31198    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjsmall:prototype_statusneither -0.933181   0.729939  -1.278  0.20109    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjsmall:prototype_statussmall   -2.629010   0.883404  -2.976  0.00292 ** </t>
+  </si>
+  <si>
+    <t>0|1 -12.2371     1.0238 -11.953</t>
+  </si>
+  <si>
+    <t>1|2  -3.7337     0.7931  -4.708</t>
+  </si>
+  <si>
+    <t>2|3   3.1447     0.7838   4.012</t>
+  </si>
+  <si>
+    <t>3|4   8.7395     0.8208  10.647</t>
+  </si>
+  <si>
+    <t>4|5  12.7812     0.8630  14.810</t>
+  </si>
+  <si>
+    <t>5|6  16.3069     1.0143  16.077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (1 + adj | noun) + (1 | subid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> link  threshold nobs logLik   AIC     niter      max.grad cond.H </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> logit flexible  2087 -1900.44 3834.87 1494(7232) 5.57e-04 1.4e+05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> subid  (Intercept) 8.40696  2.8995          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> noun   (Intercept) 0.02985  0.1728          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall    0.10955  0.3310   -1.000 </t>
+  </si>
+  <si>
+    <t>adjsmall                          3.300099   0.245569  13.439  &lt; 2e-16 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prototype_statusneither           0.190840   0.203797   0.936   0.3491    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prototype_statussmall             0.491606   0.203822   2.412   0.0159 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dirdesc                          -0.077089   0.091521  -0.842   0.3996    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quest_order                       0.001946   0.003315   0.587   0.5572    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjsmall:prototype_statusneither -0.483092   0.324565  -1.488   0.1366    </t>
+  </si>
+  <si>
+    <t>adjsmall:prototype_statussmall   -1.307171   0.325718  -4.013 5.99e-05 ***</t>
+  </si>
+  <si>
+    <t>0|1  -9.7242     0.6837 -14.224</t>
+  </si>
+  <si>
+    <t>1|2  -2.2786     0.4821  -4.726</t>
+  </si>
+  <si>
+    <t>2|3   1.9161     0.4769   4.018</t>
+  </si>
+  <si>
+    <t>3|4   5.1307     0.4922  10.424</t>
+  </si>
+  <si>
+    <t>4|5   7.5224     0.5117  14.700</t>
+  </si>
+  <si>
+    <t>5|6  10.1775     0.6688  15.218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formula: fac_num_checked ~ adj * mean + dir + quest_order + (1 + adj |  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> logit flexible  2087 -1319.37 2672.75 1657(21808) 1.94e-02 6.9e+05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> subid  (Intercept) 17.5920  4.1943          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall    22.7192  4.7665   -0.308 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> noun   (Intercept)  0.2082  0.4563          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall     0.8465  0.9201   -1.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">               Estimate Std. Error z value Pr(&gt;|z|)   </t>
+  </si>
+  <si>
+    <t>adjsmall       2.861099   0.898781   3.183  0.00146 **</t>
+  </si>
+  <si>
+    <t>mean          -0.018682   0.006960  -2.684  0.00727 **</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dirdesc       -0.074536   0.113605  -0.656  0.51176   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quest_order    0.005404   0.004208   1.284  0.19910   </t>
+  </si>
+  <si>
+    <t>adjsmall:mean  0.041222   0.012685   3.250  0.00115 **</t>
+  </si>
+  <si>
+    <t>0|1 -12.4064     0.9400 -13.198</t>
+  </si>
+  <si>
+    <t>1|2  -4.7378     0.7433  -6.374</t>
+  </si>
+  <si>
+    <t>2|3   1.8657     0.7152   2.609</t>
+  </si>
+  <si>
+    <t>3|4   7.1770     0.7407   9.690</t>
+  </si>
+  <si>
+    <t>4|5  10.8288     0.7759  13.956</t>
+  </si>
+  <si>
+    <t>5|6  13.8778     0.9008  15.407</t>
+  </si>
+  <si>
+    <t>m.bunny.norm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    noun) + (1 + adj * mean | subid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> logit flexible  2087 -1502.18 3052.36 4369(34304) 3.21e+02 NaN   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Groups Name          Variance  Std.Dev. Corr                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> subid  (Intercept)   4.377e+00 2.092194                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall      4.629e+00 2.151427  0.045               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        mean          9.511e-05 0.009752  0.039 -0.955        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall:mean 3.111e-04 0.017639 -0.109  0.901 -0.989 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> noun   (Intercept)   2.361e-02 0.153662                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall      4.522e-01 0.672426 -0.393               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">               Estimate Std. Error z value Pr(&gt;|z|)</t>
+  </si>
+  <si>
+    <t>adjsmall       0.387655         NA      NA       NA</t>
+  </si>
+  <si>
+    <t>mean          -0.016141         NA      NA       NA</t>
+  </si>
+  <si>
+    <t>dirdesc       -0.049981         NA      NA       NA</t>
+  </si>
+  <si>
+    <t>quest_order    0.001995         NA      NA       NA</t>
+  </si>
+  <si>
+    <t>adjsmall:mean  0.054846         NA      NA       NA</t>
+  </si>
+  <si>
+    <t>0|1  -7.3663         NA      NA</t>
+  </si>
+  <si>
+    <t>1|2  -3.5290         NA      NA</t>
+  </si>
+  <si>
+    <t>2|3   0.5949         NA      NA</t>
+  </si>
+  <si>
+    <t>3|4   3.8827         NA      NA</t>
+  </si>
+  <si>
+    <t>4|5   6.3294         NA      NA</t>
+  </si>
+  <si>
+    <t>5|6   7.8227         NA      NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> logit flexible  2087 -1282.99 2639.98 6974(68477) 1.52e+00 1.9e+05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> subid  (Intercept)           17.9768  4.2399                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall              16.6808  4.0842   -0.121                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        protrbig               1.0160  1.0080    0.175 -0.999                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        protrneither           0.8160  0.9033    0.283 -0.692  0.702               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall:protrbig      5.2135  2.2833   -0.401  0.752 -0.768 -0.631        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall:protrneither  2.5946  1.6108   -0.478  0.625 -0.646 -0.724  0.959 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> noun   (Intercept)            0.2664  0.5161                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        adjsmall               0.8730  0.9344   -1.000                             </t>
+  </si>
+  <si>
+    <t>adjsmall               3.190221   0.812460   3.927 8.61e-05 ***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protrbig              -1.055141   0.465672  -2.266  0.02346 *  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">protrneither          -0.625374   0.457106  -1.368  0.17128    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dirdesc               -0.069567   0.116229  -0.599  0.54948    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quest_order            0.004767   0.004339   1.099  0.27197    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjsmall:protrbig      2.598229   0.814821   3.189  0.00143 ** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjsmall:protrneither  1.649848   0.773322   2.133  0.03289 *  </t>
+  </si>
+  <si>
+    <t>0|1 -12.7395     0.9916 -12.848</t>
+  </si>
+  <si>
+    <t>1|2  -4.6311     0.7574  -6.114</t>
+  </si>
+  <si>
+    <t>2|3   2.2203     0.7328   3.030</t>
+  </si>
+  <si>
+    <t>3|4   7.7519     0.7679  10.095</t>
+  </si>
+  <si>
+    <t>4|5  11.7923     0.8141  14.486</t>
+  </si>
+  <si>
+    <t>5|6  15.2728     0.9717  15.717</t>
   </si>
 </sst>
 </file>
@@ -1610,7 +1962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1681,6 +2033,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1997,10 +2365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF62151A-946C-42E6-8483-514F8E125444}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,43 +2524,43 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>19</v>
+        <v>476</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>17</v>
+        <v>477</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>478</v>
+      </c>
+      <c r="D4" s="41">
+        <v>6.5099999999999994E-8</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="G4" s="15">
+        <v>3.1699999999999999E-2</v>
       </c>
       <c r="H4" s="13">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="17">
-        <v>3181.94</v>
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="I4" s="38">
+        <v>0.311</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="L4" s="14">
+        <v>2.9199999999999999E-3</v>
+      </c>
+      <c r="M4" s="27">
+        <v>2613.2600000000002</v>
       </c>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
@@ -2203,43 +2571,43 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>19</v>
+        <v>476</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="30">
-        <v>2.26E-6</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0.6</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>17</v>
+        <v>479</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>480</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="H5" s="13">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="I5" s="13">
-        <v>0.84599999999999997</v>
-      </c>
-      <c r="J5" s="13">
-        <v>0.65</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="12">
-        <v>3185.65</v>
+        <v>0.39960000000000001</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0.55720000000000003</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0.1366</v>
+      </c>
+      <c r="L5" s="41">
+        <v>5.9899999999999999E-5</v>
+      </c>
+      <c r="M5" s="23">
+        <v>3834.87</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
@@ -2250,27 +2618,43 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>143</v>
+        <v>476</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="29">
-        <v>2996.11</v>
+        <v>481</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>482</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1.4599999999999999E-3</v>
+      </c>
+      <c r="E6" s="14">
+        <v>7.2700000000000004E-3</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.51175999999999999</v>
+      </c>
+      <c r="I6" s="38">
+        <v>0.1991</v>
+      </c>
+      <c r="J6" s="35">
+        <v>1.15E-3</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="36">
+        <v>2672.75</v>
       </c>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
@@ -2284,43 +2668,43 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>259</v>
+        <v>21</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="D7" s="30">
-        <v>9.8100000000000002E-10</v>
+        <v>22</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="15">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G7" s="20">
-        <v>9.7000000000000003E-2</v>
+      <c r="F7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="H7" s="13">
-        <v>0.73699999999999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="I7" s="13">
-        <v>0.21099999999999999</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="14">
-        <v>7.6E-3</v>
-      </c>
-      <c r="L7" s="14">
-        <v>9.7000000000000003E-3</v>
-      </c>
-      <c r="M7" s="29">
-        <v>3201.55</v>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="17">
+        <v>3181.94</v>
       </c>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
@@ -2331,19 +2715,19 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>195</v>
+        <v>24</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" s="18">
-        <v>1E-3</v>
-      </c>
-      <c r="E8" s="15">
-        <v>1.6E-2</v>
+        <v>25</v>
+      </c>
+      <c r="D8" s="30">
+        <v>2.26E-6</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.6</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>17</v>
@@ -2352,22 +2736,22 @@
         <v>17</v>
       </c>
       <c r="H8" s="13">
-        <v>0.73</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="I8" s="13">
-        <v>0.20599999999999999</v>
-      </c>
-      <c r="J8" s="18">
-        <v>3.7599999999999998E-4</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="29">
-        <v>3195.92</v>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="12">
+        <v>3185.65</v>
       </c>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
@@ -2378,43 +2762,27 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" s="18">
-        <v>1E-4</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0.32200000000000001</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="14">
-        <v>7.9000000000000008E-3</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="13">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="L9" s="13">
-        <v>0.26</v>
-      </c>
-      <c r="M9" s="27">
-        <v>3865.88</v>
+        <v>145</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="29">
+        <v>2996.11</v>
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
@@ -2425,43 +2793,43 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>215</v>
+        <v>259</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="20">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0.14560000000000001</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="J10" s="20">
-        <v>6.8500000000000005E-2</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="23">
-        <v>3865.97</v>
+        <v>260</v>
+      </c>
+      <c r="D10" s="30">
+        <v>9.8100000000000002E-10</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="15">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G10" s="20">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="14">
+        <v>7.6E-3</v>
+      </c>
+      <c r="L10" s="14">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="M10" s="29">
+        <v>3201.55</v>
       </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -2470,19 +2838,19 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>17</v>
+        <v>196</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1.6E-2</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>17</v>
@@ -2490,14 +2858,14 @@
       <c r="G11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>17</v>
+      <c r="H11" s="13">
+        <v>0.73</v>
       </c>
       <c r="I11" s="13">
-        <v>0.68899999999999995</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>17</v>
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="J11" s="18">
+        <v>3.7599999999999998E-4</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>17</v>
@@ -2505,8 +2873,8 @@
       <c r="L11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="17">
-        <v>4069.6</v>
+      <c r="M11" s="29">
+        <v>3195.92</v>
       </c>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
@@ -2515,43 +2883,43 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>236</v>
+        <v>148</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D12" s="15">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>17</v>
+        <v>149</v>
+      </c>
+      <c r="D12" s="18">
+        <v>1E-4</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.32200000000000001</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="13">
-        <v>0.70099999999999996</v>
-      </c>
-      <c r="J12" s="13">
-        <v>0.63600000000000001</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="12">
-        <v>4072.43</v>
+      <c r="I12" s="14">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="13">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="L12" s="13">
+        <v>0.26</v>
+      </c>
+      <c r="M12" s="27">
+        <v>3865.88</v>
       </c>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
@@ -2560,19 +2928,19 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.16600000000000001</v>
+        <v>216</v>
+      </c>
+      <c r="D13" s="20">
+        <v>7.7200000000000005E-2</v>
       </c>
       <c r="E13" s="13">
-        <v>0.89100000000000001</v>
+        <v>0.14560000000000001</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>17</v>
@@ -2583,11 +2951,11 @@
       <c r="H13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="13">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="J13" s="13">
-        <v>0.63649999999999995</v>
+      <c r="I13" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="J13" s="20">
+        <v>6.8500000000000005E-2</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>17</v>
@@ -2595,8 +2963,8 @@
       <c r="L13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="12">
-        <v>4084.14</v>
+      <c r="M13" s="23">
+        <v>3865.97</v>
       </c>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
@@ -2605,43 +2973,43 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>313</v>
+        <v>175</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>314</v>
+        <v>176</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>315</v>
+        <v>23</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="15">
-        <v>4.3900000000000002E-2</v>
-      </c>
-      <c r="G14" s="30">
-        <v>7.1999999999999999E-7</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0.95799999999999996</v>
+      <c r="F14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="I14" s="13">
-        <v>0.503</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="15">
-        <v>1.38E-2</v>
-      </c>
-      <c r="L14" s="30">
-        <v>8.5E-9</v>
-      </c>
-      <c r="M14" s="23">
-        <v>12071.77</v>
+      <c r="K14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="17">
+        <v>4069.6</v>
       </c>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
@@ -2650,19 +3018,19 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>316</v>
+        <v>236</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="D15" s="30">
-        <v>4.7999999999999998E-6</v>
-      </c>
-      <c r="E15" s="30">
-        <v>3.9799999999999998E-5</v>
+        <v>217</v>
+      </c>
+      <c r="D15" s="15">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.86299999999999999</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>17</v>
@@ -2670,14 +3038,14 @@
       <c r="G15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="13">
-        <v>0.95599999999999996</v>
+      <c r="H15" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="I15" s="13">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="J15" s="22">
-        <v>2.1399999999999998E-6</v>
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0.63600000000000001</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>17</v>
@@ -2685,8 +3053,8 @@
       <c r="L15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="27">
-        <v>12071.05</v>
+      <c r="M15" s="12">
+        <v>4072.43</v>
       </c>
       <c r="N15" s="12" t="s">
         <v>475</v>
@@ -2696,84 +3064,134 @@
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+      <c r="A16" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="13">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0.63649999999999995</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16" s="12">
+        <v>4084.14</v>
+      </c>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
+      <c r="A17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="15">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="G17" s="30">
+        <v>7.1999999999999999E-7</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0.503</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="15">
+        <v>1.38E-2</v>
+      </c>
+      <c r="L17" s="30">
+        <v>8.5E-9</v>
+      </c>
+      <c r="M17" s="23">
+        <v>12071.77</v>
+      </c>
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="M18" s="31" t="s">
-        <v>20</v>
+      <c r="A18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="D18" s="30">
+        <v>4.7999999999999998E-6</v>
+      </c>
+      <c r="E18" s="30">
+        <v>3.9799999999999998E-5</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="13">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="I18" s="13">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="J18" s="22">
+        <v>2.1399999999999998E-6</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="27">
+        <v>12071.05</v>
       </c>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
@@ -2781,134 +3199,84 @@
       <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="D19" s="14">
-        <v>2E-3</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="15">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="G19" s="14">
-        <v>5.2500000000000003E-3</v>
-      </c>
-      <c r="H19" s="13">
-        <v>0.91</v>
-      </c>
-      <c r="I19" s="30">
-        <v>9.1100000000000004E-7</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="15">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="L19" s="14">
-        <v>1.42E-3</v>
-      </c>
-      <c r="M19" s="23">
-        <v>3222.97</v>
-      </c>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>366</v>
-      </c>
-      <c r="D20" s="30">
-        <v>9.1600000000000006E-9</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="33">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="G20" s="30">
-        <v>7.1900000000000002E-7</v>
-      </c>
-      <c r="H20" s="34">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="I20" s="34">
-        <v>0.503</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="28">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="L20" s="30">
-        <v>8.4900000000000003E-9</v>
-      </c>
-      <c r="M20" s="23">
-        <v>12071.77</v>
-      </c>
+      <c r="A20" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>406</v>
-      </c>
-      <c r="D21" s="30">
-        <v>7.25E-5</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="34">
-        <v>0.89600000000000002</v>
-      </c>
-      <c r="G21" s="34">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="H21" s="13">
-        <v>0.86</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0.26800000000000002</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="13">
-        <v>0.95850000000000002</v>
-      </c>
-      <c r="L21" s="20">
-        <v>9.0800000000000006E-2</v>
-      </c>
-      <c r="M21" s="23">
-        <v>2989.73</v>
+      <c r="A21" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
@@ -2917,43 +3285,43 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>430</v>
+        <v>332</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>336</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>431</v>
-      </c>
-      <c r="D22" s="30">
-        <v>2.69E-5</v>
+        <v>337</v>
+      </c>
+      <c r="D22" s="14">
+        <v>2E-3</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="13">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="G22" s="20">
-        <v>9.7000000000000003E-2</v>
+      <c r="F22" s="15">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G22" s="14">
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="H22" s="13">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="I22" s="13">
-        <v>0.21</v>
+        <v>0.91</v>
+      </c>
+      <c r="I22" s="30">
+        <v>9.1100000000000004E-7</v>
       </c>
       <c r="J22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="13">
-        <v>0.93700000000000006</v>
+      <c r="K22" s="15">
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="L22" s="14">
-        <v>9.6799999999999994E-3</v>
+        <v>1.42E-3</v>
       </c>
       <c r="M22" s="23">
-        <v>3201.55</v>
+        <v>3222.97</v>
       </c>
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
@@ -2962,43 +3330,43 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>147</v>
+        <v>3</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>449</v>
+        <v>365</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>450</v>
-      </c>
-      <c r="D23" s="35">
-        <v>5.6699999999999997E-3</v>
+        <v>366</v>
+      </c>
+      <c r="D23" s="30">
+        <v>9.1600000000000006E-9</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="13">
-        <v>0.89600000000000002</v>
-      </c>
-      <c r="G23" s="13">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="14">
-        <v>7.9900000000000006E-3</v>
+      <c r="F23" s="33">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="G23" s="30">
+        <v>7.1900000000000002E-7</v>
+      </c>
+      <c r="H23" s="34">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="I23" s="34">
+        <v>0.503</v>
       </c>
       <c r="J23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="13">
-        <v>0.87580000000000002</v>
-      </c>
-      <c r="L23" s="13">
-        <v>0.26050000000000001</v>
+      <c r="K23" s="28">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="L23" s="30">
+        <v>8.4900000000000003E-9</v>
       </c>
       <c r="M23" s="23">
-        <v>3865.88</v>
+        <v>12071.77</v>
       </c>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
@@ -3006,61 +3374,225 @@
       <c r="Q23" s="12"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
+      <c r="A24" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>484</v>
+      </c>
+      <c r="D24" s="41">
+        <v>8.6100000000000006E-5</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="34">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G24" s="39">
+        <v>2.3460000000000002E-2</v>
+      </c>
+      <c r="H24" s="34">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I24" s="34">
+        <v>0.27189999999999998</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="39">
+        <v>3.2890000000000003E-2</v>
+      </c>
+      <c r="L24" s="35">
+        <v>1.4300000000000001E-3</v>
+      </c>
+      <c r="M24" s="23">
+        <v>3834.87</v>
+      </c>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
+      <c r="A25" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="D25" s="30">
+        <v>7.25E-5</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="34">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="G25" s="34">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0.86</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="13">
+        <v>0.95850000000000002</v>
+      </c>
+      <c r="L25" s="20">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="M25" s="23">
+        <v>2989.73</v>
+      </c>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
+      <c r="A26" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>431</v>
+      </c>
+      <c r="D26" s="30">
+        <v>2.69E-5</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="G26" s="20">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="H26" s="13">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="I26" s="13">
+        <v>0.21</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="13">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="L26" s="14">
+        <v>9.6799999999999994E-3</v>
+      </c>
+      <c r="M26" s="23">
+        <v>3201.55</v>
+      </c>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>450</v>
+      </c>
+      <c r="D27" s="35">
+        <v>5.6699999999999997E-3</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="13">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="14">
+        <v>7.9900000000000006E-3</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="13">
+        <v>0.87580000000000002</v>
+      </c>
+      <c r="L27" s="13">
+        <v>0.26050000000000001</v>
+      </c>
+      <c r="M27" s="23">
+        <v>3865.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3070,10 +3602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446F4D70-7C12-4200-99E8-BFE4A4C2375D}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3084,7 +3616,8 @@
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="11" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -3226,194 +3759,201 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>19</v>
+        <v>476</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="28">
-        <v>-8.5120000000000005</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>17</v>
+        <v>477</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>478</v>
+      </c>
+      <c r="D4" s="18">
+        <v>5.4039999999999999</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G4" s="15">
+        <v>2.1480000000000001</v>
       </c>
       <c r="H4" s="13">
-        <v>1.482</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0.182</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="17">
-        <v>3181.94</v>
+        <v>-0.70699999999999996</v>
+      </c>
+      <c r="I4" s="38">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="13">
+        <v>-1.278</v>
+      </c>
+      <c r="L4" s="14">
+        <v>-2.976</v>
+      </c>
+      <c r="M4" s="27">
+        <v>2613.2600000000002</v>
       </c>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
-      <c r="P4" s="18" t="s">
-        <v>306</v>
-      </c>
+      <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>19</v>
+        <v>476</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="26">
-        <v>-4.7290000000000001</v>
-      </c>
-      <c r="E5" s="13">
-        <v>-0.52400000000000002</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>17</v>
+        <v>479</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>480</v>
+      </c>
+      <c r="D5" s="18">
+        <v>13.439</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="G5" s="15">
+        <v>2.4119999999999999</v>
       </c>
       <c r="H5" s="13">
-        <v>1.4790000000000001</v>
-      </c>
-      <c r="I5" s="13">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="J5" s="13">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="12">
-        <v>3185.65</v>
+        <v>-0.84199999999999997</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="13">
+        <v>-1.488</v>
+      </c>
+      <c r="L5" s="18">
+        <v>-4.0129999999999999</v>
+      </c>
+      <c r="M5" s="23">
+        <v>3834.87</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
-      <c r="P5" s="14" t="s">
-        <v>307</v>
-      </c>
+      <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>143</v>
+        <v>476</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="29">
-        <v>2996.11</v>
-      </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q6" s="12"/>
-      <c r="R6" t="s">
-        <v>312</v>
-      </c>
+        <v>481</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>482</v>
+      </c>
+      <c r="D6" s="14">
+        <v>3.1829999999999998</v>
+      </c>
+      <c r="E6" s="14">
+        <v>-2.6840000000000002</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="13">
+        <v>-0.65600000000000003</v>
+      </c>
+      <c r="I6" s="38">
+        <v>1.284</v>
+      </c>
+      <c r="J6" s="35">
+        <v>3.25</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="36">
+        <v>2672.75</v>
+      </c>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>259</v>
+        <v>21</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="D7" s="26">
-        <v>6.1120000000000001</v>
+        <v>22</v>
+      </c>
+      <c r="D7" s="28">
+        <v>-8.5120000000000005</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="15">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="G7" s="20">
-        <v>1.657</v>
+      <c r="F7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="H7" s="13">
-        <v>-0.33500000000000002</v>
+        <v>1.482</v>
       </c>
       <c r="I7" s="13">
-        <v>-1.2509999999999999</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="14">
-        <v>-2.669</v>
-      </c>
-      <c r="L7" s="14">
-        <v>-2.5870000000000002</v>
-      </c>
-      <c r="M7" s="29">
-        <v>3201.55</v>
+        <v>0.182</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="17">
+        <v>3181.94</v>
       </c>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
-      <c r="P7" s="20" t="s">
-        <v>309</v>
+      <c r="P7" s="18" t="s">
+        <v>306</v>
       </c>
       <c r="Q7" s="12"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>195</v>
+        <v>24</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" s="18">
-        <v>3.2890000000000001</v>
-      </c>
-      <c r="E8" s="15">
-        <v>-2.41</v>
+        <v>25</v>
+      </c>
+      <c r="D8" s="26">
+        <v>-4.7290000000000001</v>
+      </c>
+      <c r="E8" s="13">
+        <v>-0.52400000000000002</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>17</v>
@@ -3422,137 +3962,126 @@
         <v>17</v>
       </c>
       <c r="H8" s="13">
-        <v>-0.33900000000000002</v>
+        <v>1.4790000000000001</v>
       </c>
       <c r="I8" s="13">
-        <v>-1.2649999999999999</v>
-      </c>
-      <c r="J8" s="18">
-        <v>3.5569999999999999</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="29">
-        <v>3195.92</v>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="12">
+        <v>3185.65</v>
       </c>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
-      <c r="P8" s="17" t="s">
-        <v>310</v>
+      <c r="P8" s="14" t="s">
+        <v>307</v>
       </c>
       <c r="Q8" s="12"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" s="18">
-        <v>3.782</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0.84299999999999997</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="14">
-        <v>2.653</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="13">
-        <v>-1.2669999999999999</v>
-      </c>
-      <c r="L9" s="13">
-        <v>-1.125</v>
-      </c>
-      <c r="M9" s="27">
-        <v>3865.88</v>
+        <v>145</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="29">
+        <v>2996.11</v>
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
-      <c r="P9" s="21" t="s">
-        <v>305</v>
+      <c r="P9" s="15" t="s">
+        <v>308</v>
       </c>
       <c r="Q9" s="12"/>
+      <c r="R9" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>215</v>
+        <v>259</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="20">
-        <v>1.7669999999999999</v>
-      </c>
-      <c r="E10" s="13">
-        <v>-1.4550000000000001</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="15">
-        <v>2.52</v>
-      </c>
-      <c r="J10" s="20">
-        <v>1.8220000000000001</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="23">
-        <v>3865.97</v>
+        <v>260</v>
+      </c>
+      <c r="D10" s="26">
+        <v>6.1120000000000001</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="15">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G10" s="20">
+        <v>1.657</v>
+      </c>
+      <c r="H10" s="13">
+        <v>-0.33500000000000002</v>
+      </c>
+      <c r="I10" s="13">
+        <v>-1.2509999999999999</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="14">
+        <v>-2.669</v>
+      </c>
+      <c r="L10" s="14">
+        <v>-2.5870000000000002</v>
+      </c>
+      <c r="M10" s="29">
+        <v>3201.55</v>
       </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
+      <c r="P10" s="20" t="s">
+        <v>309</v>
+      </c>
       <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="28">
-        <v>-10.099</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>17</v>
+        <v>196</v>
+      </c>
+      <c r="D11" s="18">
+        <v>3.2890000000000001</v>
+      </c>
+      <c r="E11" s="15">
+        <v>-2.41</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>17</v>
@@ -3560,14 +4089,14 @@
       <c r="G11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>17</v>
+      <c r="H11" s="13">
+        <v>-0.33900000000000002</v>
       </c>
       <c r="I11" s="13">
-        <v>-0.40100000000000002</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>17</v>
+        <v>-1.2649999999999999</v>
+      </c>
+      <c r="J11" s="18">
+        <v>3.5569999999999999</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>17</v>
@@ -3575,74 +4104,78 @@
       <c r="L11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="17">
-        <v>4069.6</v>
+      <c r="M11" s="29">
+        <v>3195.92</v>
       </c>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
+      <c r="P11" s="40" t="s">
+        <v>485</v>
+      </c>
       <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>236</v>
+        <v>148</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D12" s="15">
-        <v>-2.387</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>17</v>
+        <v>149</v>
+      </c>
+      <c r="D12" s="18">
+        <v>3.782</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.99099999999999999</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="13">
-        <v>-0.38300000000000001</v>
-      </c>
-      <c r="J12" s="13">
-        <v>-0.47399999999999998</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="12">
-        <v>4072.43</v>
+      <c r="I12" s="14">
+        <v>2.653</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="13">
+        <v>-1.2669999999999999</v>
+      </c>
+      <c r="L12" s="13">
+        <v>-1.125</v>
+      </c>
+      <c r="M12" s="27">
+        <v>3865.88</v>
       </c>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
+      <c r="P12" s="17" t="s">
+        <v>310</v>
+      </c>
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="D13" s="15">
-        <v>-2.3959999999999999</v>
+        <v>216</v>
+      </c>
+      <c r="D13" s="20">
+        <v>1.7669999999999999</v>
       </c>
       <c r="E13" s="13">
-        <v>0.13700000000000001</v>
+        <v>-1.4550000000000001</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>17</v>
@@ -3653,11 +4186,11 @@
       <c r="H13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="13">
-        <v>-0.36</v>
-      </c>
-      <c r="J13" s="13">
-        <v>-0.47299999999999998</v>
+      <c r="I13" s="15">
+        <v>2.52</v>
+      </c>
+      <c r="J13" s="20">
+        <v>1.8220000000000001</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>17</v>
@@ -3665,76 +4198,76 @@
       <c r="L13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="12">
-        <v>4084.14</v>
+      <c r="M13" s="23">
+        <v>3865.97</v>
       </c>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
+      <c r="P13" s="21" t="s">
+        <v>305</v>
+      </c>
       <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>313</v>
+        <v>175</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>315</v>
+        <v>176</v>
+      </c>
+      <c r="D14" s="28">
+        <v>-10.099</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="15">
-        <v>4.3900000000000002E-2</v>
-      </c>
-      <c r="G14" s="30">
-        <v>7.1999999999999999E-7</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0.95799999999999996</v>
+      <c r="F14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="I14" s="13">
-        <v>0.503</v>
+        <v>-0.40100000000000002</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="15">
-        <v>1.38E-2</v>
-      </c>
-      <c r="L14" s="30">
-        <v>8.5E-9</v>
-      </c>
-      <c r="M14" s="23">
-        <v>12071.77</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>474</v>
-      </c>
+      <c r="K14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="17">
+        <v>4069.6</v>
+      </c>
+      <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>316</v>
+        <v>236</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="D15" s="30">
-        <v>4.7999999999999998E-6</v>
-      </c>
-      <c r="E15" s="30">
-        <v>3.9799999999999998E-5</v>
+        <v>217</v>
+      </c>
+      <c r="D15" s="15">
+        <v>-2.387</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.17299999999999999</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>17</v>
@@ -3742,14 +4275,14 @@
       <c r="G15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="13">
-        <v>0.95599999999999996</v>
+      <c r="H15" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="I15" s="13">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="J15" s="22">
-        <v>2.1399999999999998E-6</v>
+        <v>-0.38300000000000001</v>
+      </c>
+      <c r="J15" s="13">
+        <v>-0.47399999999999998</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>17</v>
@@ -3757,30 +4290,54 @@
       <c r="L15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="23">
-        <v>12071.05</v>
-      </c>
-      <c r="N15" s="12" t="s">
-        <v>474</v>
-      </c>
+      <c r="M15" s="12">
+        <v>4072.43</v>
+      </c>
+      <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
+      <c r="A16" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" s="15">
+        <v>-2.3959999999999999</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="13">
+        <v>-0.36</v>
+      </c>
+      <c r="J16" s="13">
+        <v>-0.47299999999999998</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16" s="12">
+        <v>4084.14</v>
+      </c>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
@@ -3788,108 +4345,112 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+        <v>3</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="15">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="G17" s="30">
+        <v>7.1999999999999999E-7</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0.503</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="15">
+        <v>1.38E-2</v>
+      </c>
+      <c r="L17" s="30">
+        <v>8.5E-9</v>
+      </c>
+      <c r="M17" s="23">
+        <v>12071.77</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>474</v>
+      </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="M18" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="N18" s="12"/>
+      <c r="A18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="D18" s="30">
+        <v>4.7999999999999998E-6</v>
+      </c>
+      <c r="E18" s="30">
+        <v>3.9799999999999998E-5</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="13">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="I18" s="13">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="J18" s="22">
+        <v>2.1399999999999998E-6</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="23">
+        <v>12071.05</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>474</v>
+      </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="D19" s="14">
-        <v>3.08</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="15">
-        <v>-2.032</v>
-      </c>
-      <c r="G19" s="14">
-        <v>-2.7909999999999999</v>
-      </c>
-      <c r="H19" s="12">
-        <v>-0.112</v>
-      </c>
-      <c r="I19" s="26">
-        <v>-4.91</v>
-      </c>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="K19" s="15">
-        <v>2.0819999999999999</v>
-      </c>
-      <c r="L19" s="14">
-        <v>3.19</v>
-      </c>
-      <c r="M19" s="23">
-        <v>3222.97</v>
-      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
@@ -3897,90 +4458,64 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>366</v>
-      </c>
-      <c r="D20" s="26">
-        <v>5.7460000000000004</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="33">
-        <v>-2.9550000000000001</v>
-      </c>
-      <c r="G20" s="28">
-        <v>-4.9560000000000004</v>
-      </c>
-      <c r="H20" s="34">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="I20" s="34">
-        <v>0.67</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="28">
-        <v>3.3130000000000002</v>
-      </c>
-      <c r="L20" s="26">
-        <v>5.758</v>
-      </c>
-      <c r="M20" s="23">
-        <v>12071.77</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>474</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>406</v>
-      </c>
-      <c r="D21" s="26">
-        <v>3.968</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="34">
-        <v>0.13</v>
-      </c>
-      <c r="G21" s="34">
-        <v>-1.2889999999999999</v>
-      </c>
-      <c r="H21" s="13">
-        <v>-0.17599999999999999</v>
-      </c>
-      <c r="I21" s="13">
-        <v>-1.1080000000000001</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="13">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="L21" s="18">
-        <v>1.6910000000000001</v>
-      </c>
-      <c r="M21" s="23">
-        <v>2989.73</v>
+      <c r="A21" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
@@ -3989,43 +4524,43 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>430</v>
+        <v>332</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>336</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>431</v>
-      </c>
-      <c r="D22" s="26">
-        <v>4.1980000000000004</v>
+        <v>337</v>
+      </c>
+      <c r="D22" s="14">
+        <v>3.08</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="13">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="G22" s="20">
-        <v>-1.657</v>
+      <c r="F22" s="15">
+        <v>-2.032</v>
+      </c>
+      <c r="G22" s="14">
+        <v>-2.7909999999999999</v>
       </c>
       <c r="H22" s="13">
-        <v>-0.33500000000000002</v>
-      </c>
-      <c r="I22" s="13">
-        <v>-1.2509999999999999</v>
+        <v>-0.112</v>
+      </c>
+      <c r="I22" s="26">
+        <v>-4.91</v>
       </c>
       <c r="J22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="13">
-        <v>-7.9000000000000001E-2</v>
+      <c r="K22" s="15">
+        <v>2.0819999999999999</v>
       </c>
       <c r="L22" s="14">
-        <v>2.5870000000000002</v>
+        <v>3.19</v>
       </c>
       <c r="M22" s="23">
-        <v>3201.55</v>
+        <v>3222.97</v>
       </c>
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
@@ -4034,67 +4569,249 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>147</v>
+        <v>3</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>449</v>
+        <v>365</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>450</v>
-      </c>
-      <c r="D23" s="35">
-        <v>2.766</v>
+        <v>366</v>
+      </c>
+      <c r="D23" s="26">
+        <v>5.7460000000000004</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="13">
-        <v>-0.13</v>
-      </c>
-      <c r="G23" s="13">
-        <v>-0.99099999999999999</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="14">
-        <v>2.653</v>
+      <c r="F23" s="33">
+        <v>-2.9550000000000001</v>
+      </c>
+      <c r="G23" s="28">
+        <v>-4.9560000000000004</v>
+      </c>
+      <c r="H23" s="34">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="I23" s="34">
+        <v>0.67</v>
       </c>
       <c r="J23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="13">
-        <v>-0.156</v>
-      </c>
-      <c r="L23" s="13">
-        <v>1.125</v>
+      <c r="K23" s="28">
+        <v>3.3130000000000002</v>
+      </c>
+      <c r="L23" s="26">
+        <v>5.758</v>
       </c>
       <c r="M23" s="23">
-        <v>3865.88</v>
-      </c>
-      <c r="N23" s="12"/>
+        <v>12071.77</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>474</v>
+      </c>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
+      <c r="A24" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>484</v>
+      </c>
+      <c r="D24" s="26">
+        <v>3.927</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="34">
+        <v>-1.3680000000000001</v>
+      </c>
+      <c r="G24" s="39">
+        <v>-2.266</v>
+      </c>
+      <c r="H24" s="34">
+        <v>-0.59899999999999998</v>
+      </c>
+      <c r="I24" s="34">
+        <v>1.099</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="39">
+        <v>2.133</v>
+      </c>
+      <c r="L24" s="35">
+        <v>3.1890000000000001</v>
+      </c>
+      <c r="M24" s="23">
+        <v>3834.87</v>
+      </c>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="D25" s="26">
+        <v>3.968</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="34">
+        <v>0.13</v>
+      </c>
+      <c r="G25" s="34">
+        <v>-1.2889999999999999</v>
+      </c>
+      <c r="H25" s="13">
+        <v>-0.17599999999999999</v>
+      </c>
+      <c r="I25" s="13">
+        <v>-1.1080000000000001</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="13">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="L25" s="18">
+        <v>1.6910000000000001</v>
+      </c>
+      <c r="M25" s="23">
+        <v>2989.73</v>
+      </c>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+    </row>
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>431</v>
+      </c>
+      <c r="D26" s="26">
+        <v>4.1980000000000004</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="G26" s="20">
+        <v>-1.657</v>
+      </c>
+      <c r="H26" s="13">
+        <v>-0.33500000000000002</v>
+      </c>
+      <c r="I26" s="13">
+        <v>-1.2509999999999999</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="13">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="L26" s="14">
+        <v>2.5870000000000002</v>
+      </c>
+      <c r="M26" s="23">
+        <v>3201.55</v>
+      </c>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>450</v>
+      </c>
+      <c r="D27" s="35">
+        <v>2.766</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="13">
+        <v>-0.13</v>
+      </c>
+      <c r="G27" s="13">
+        <v>-0.99099999999999999</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="14">
+        <v>2.653</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="13">
+        <v>-0.156</v>
+      </c>
+      <c r="L27" s="13">
+        <v>1.125</v>
+      </c>
+      <c r="M27" s="23">
+        <v>3865.88</v>
+      </c>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4107,7 +4824,7 @@
   <dimension ref="A1:M124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+      <selection activeCell="S120" sqref="S120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5319,6 +6036,1028 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35448E15-EE61-4A8F-87E4-301803AD8ECA}">
+  <dimension ref="A1:J206"/>
+  <sheetViews>
+    <sheetView topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="H206" sqref="H206"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="6"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+      <c r="I164" s="6"/>
+      <c r="J164" s="6"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF64B61-BB41-454D-AB73-7D52C2DF5042}">
   <dimension ref="A1:K71"/>
   <sheetViews>
@@ -5676,7 +7415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CBF8E-AAA7-4A22-ABA8-201E023C78BF}">
   <dimension ref="A1:N196"/>
   <sheetViews>
@@ -6659,7 +8398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CBD8FFC-799E-4C6F-85C8-EB2695D9CE9D}">
   <dimension ref="A1:L114"/>
   <sheetViews>
@@ -7231,7 +8970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418E8191-8460-40B0-9F5D-15A6ACBA7ADB}">
   <dimension ref="A1:M107"/>
   <sheetViews>

</xml_diff>